<commit_message>
some unncessary lines removed
</commit_message>
<xml_diff>
--- a/search/excel.xlsx
+++ b/search/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\5. Activities\fourbeats\search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEB6BC8-BBE2-49D8-BEBD-061F23C91BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DBB2BED-B96C-4D9D-B774-2FAA26E318DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -918,7 +918,7 @@
   <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
erased and edited some lines
</commit_message>
<xml_diff>
--- a/search/excel.xlsx
+++ b/search/excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\5. Activities\fourbeats\search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CD35C9-6D62-4C80-BEB0-BA8D8E3C3692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD106E4-A643-4E9E-A0A8-C4B7E1139F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Saturday" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,9 @@
   </sheetPr>
   <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -917,8 +919,8 @@
   </sheetPr>
   <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>